<commit_message>
Add new images for apples to test
side and top view with the actual mass
will need to play around with the alpha value or
find a way to calulcate the volume with just the side
or both side and top view of apple
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99E6685D-AB1F-41BA-9CA7-3F0738C53882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0A6EA1-30A8-4D70-A18E-D597204AA03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t>apple</t>
   </si>
@@ -120,6 +121,48 @@
   </si>
   <si>
     <t>Volume of sphere</t>
+  </si>
+  <si>
+    <t>Fruit/Vegetable Experiment</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Alpha (Adjust sphere equation)</t>
+  </si>
+  <si>
+    <t>Image_File_Path</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Actual Mass (grams)</t>
+  </si>
+  <si>
+    <t>Estimated Mass (grams)</t>
+  </si>
+  <si>
+    <t>pink lady</t>
+  </si>
+  <si>
+    <t>date:24-sept-22</t>
+  </si>
+  <si>
+    <t>photo_ver</t>
   </si>
 </sst>
 </file>
@@ -151,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +213,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -392,11 +447,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,6 +618,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -777,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1625A3-6185-408F-A960-F2F45C042592}">
   <dimension ref="B1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -995,4 +1202,392 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="17.20703125" customWidth="1"/>
+    <col min="4" max="4" width="37.26171875" customWidth="1"/>
+    <col min="5" max="5" width="33.20703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="3" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="5"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="5"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="5"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="5"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="6"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="28">
+        <v>1</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23">
+        <v>264</v>
+      </c>
+      <c r="F13" s="22"/>
+      <c r="G13" s="24"/>
+      <c r="I13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="29"/>
+      <c r="B14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="31">
+        <v>264</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="32"/>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="30">
+        <v>2</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34">
+        <v>254</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="35"/>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="30"/>
+      <c r="B16" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34">
+        <v>254</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="35"/>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="28">
+        <v>3</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23">
+        <v>260</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="24"/>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="29"/>
+      <c r="B18" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="31">
+        <v>260</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="32"/>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="30">
+        <v>4</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34">
+        <v>298</v>
+      </c>
+      <c r="F19" s="33"/>
+      <c r="G19" s="35"/>
+      <c r="I19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A20" s="30"/>
+      <c r="B20" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34">
+        <v>298</v>
+      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="35"/>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="28">
+        <v>5</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23">
+        <v>237</v>
+      </c>
+      <c r="F21" s="22"/>
+      <c r="G21" s="24"/>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A22" s="29"/>
+      <c r="B22" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="31">
+        <v>237</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="32"/>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="30">
+        <v>6</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34">
+        <v>189</v>
+      </c>
+      <c r="F23" s="33"/>
+      <c r="G23" s="35"/>
+      <c r="I23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A24" s="29"/>
+      <c r="B24" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="31">
+        <v>189</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="32"/>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update excel sheet for adjustment values for apple and orange
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0A6EA1-30A8-4D70-A18E-D597204AA03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27AACA5-EEF4-474D-8F03-F9D5BA37434D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="2" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Apple" sheetId="2" r:id="rId2"/>
+    <sheet name="Orange" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="84">
   <si>
     <t>apple</t>
   </si>
@@ -153,16 +154,337 @@
     <t>Actual Mass (grams)</t>
   </si>
   <si>
-    <t>Estimated Mass (grams)</t>
-  </si>
-  <si>
     <t>pink lady</t>
   </si>
   <si>
     <t>date:24-sept-22</t>
   </si>
   <si>
-    <t>photo_ver</t>
+    <t>photo_ver (best)</t>
+  </si>
+  <si>
+    <t>Estimated Mass (grams) [Best]</t>
+  </si>
+  <si>
+    <t>(Adjustment, mass)</t>
+  </si>
+  <si>
+    <t>using sphere volume equation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.15, 146], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[3.5, 238.6]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.0, 88], [2.0, 176.8], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.15, 190]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[3.5, 506], [2.15, 311], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.065, 299]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.065, 217], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.475, 260]</t>
+    </r>
+  </si>
+  <si>
+    <t>apple 3 Side</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.475, 292], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.15, 253]</t>
+    </r>
+  </si>
+  <si>
+    <t>apple 1 side</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.475, 236], [2.15, 205], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.78, 265]</t>
+    </r>
+  </si>
+  <si>
+    <t>orange_test2.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1, 220], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.62, 357]</t>
+    </r>
+  </si>
+  <si>
+    <t>orange2_327gram.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.62, 355], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.5, 328]</t>
+    </r>
+  </si>
+  <si>
+    <t>orange3_333gram.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.5, 276], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.81, 332]</t>
+    </r>
+  </si>
+  <si>
+    <t>orange4_339gram.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.81, 293], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.1, 340]</t>
+    </r>
+  </si>
+  <si>
+    <t>examples of bad finger image segmentation and also the square block problems</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.1, 457], [1.62, 353], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.435, 312]</t>
+    </r>
+  </si>
+  <si>
+    <t>orange5_312gram_ver4.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.435, 286], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.6, 318]</t>
+    </r>
+  </si>
+  <si>
+    <t>orange6_319gram.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.6, 270], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.92, 323]</t>
+    </r>
+  </si>
+  <si>
+    <t>[1.92, 315]</t>
+  </si>
+  <si>
+    <t>:o</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>orange8_315gram.jpg</t>
+  </si>
+  <si>
+    <t>orange7_324gram.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.92, 385], [1.62, 325], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.54, 309]</t>
+    </r>
+  </si>
+  <si>
+    <t>orange9_308gram.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.54, 303], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.72, 338]</t>
+    </r>
+  </si>
+  <si>
+    <t>[1.62, 357]</t>
+  </si>
+  <si>
+    <t>[1.5, 328]</t>
+  </si>
+  <si>
+    <t>[1.81, 332]</t>
+  </si>
+  <si>
+    <t>[2.1, 340]</t>
+  </si>
+  <si>
+    <t>[1.435, 312]</t>
+  </si>
+  <si>
+    <t>[1.6, 318]</t>
+  </si>
+  <si>
+    <t>[1.92, 323]</t>
+  </si>
+  <si>
+    <t>[1.54, 309]</t>
+  </si>
+  <si>
+    <t>[1.72, 338]</t>
+  </si>
+  <si>
+    <t>orange10_338gram.jpg</t>
   </si>
 </sst>
 </file>
@@ -555,7 +877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,6 +942,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,6 +973,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,6 +995,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,6 +1024,236 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>88899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2456392</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>32807</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B485402-4D74-7784-F7EE-5B1D6064955F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="5283199"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2374901</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>105832</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1453092</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>49740</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BD25275-E677-BA84-A1F9-A3DD5FF8A48C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6443134" y="5300132"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>81915</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>169545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E92326A2-4102-76D4-22C4-8F63717A04E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="457200" y="3185160"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>260985</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D5C6C6-4638-A626-C8C4-6120EDA9E82E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6812280" y="3204210"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8076067B-620E-76E4-834C-1C9234265368}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="8751570"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1206,19 +1777,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="17.20703125" customWidth="1"/>
-    <col min="4" max="4" width="37.26171875" customWidth="1"/>
-    <col min="5" max="5" width="33.20703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.68359375" customWidth="1"/>
+    <col min="3" max="4" width="17.20703125" customWidth="1"/>
+    <col min="5" max="5" width="37.26171875" customWidth="1"/>
+    <col min="6" max="6" width="33.20703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.68359375" customWidth="1"/>
+    <col min="8" max="8" width="49.3671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1234,15 +1806,16 @@
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="16"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="4" t="s">
@@ -1251,331 +1824,360 @@
       <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="17"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="5"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="18"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="5"/>
       <c r="C6" s="9"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="18"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="5"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="18"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="5"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="18"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="19"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="26" t="s">
+      <c r="E12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="F12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="G12" s="39" t="s">
         <v>41</v>
       </c>
+      <c r="H12" s="40" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="28">
+      <c r="A13" s="30">
         <v>1</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23">
+      <c r="D13" s="24">
+        <v>3</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25">
         <v>264</v>
       </c>
-      <c r="F13" s="22"/>
       <c r="G13" s="24"/>
-      <c r="I13">
-        <v>3</v>
+      <c r="H13" s="26" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="29"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="31">
+      <c r="D14" s="21">
+        <v>1</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="34">
         <v>264</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="32"/>
-      <c r="I14">
+      <c r="G14" s="21"/>
+      <c r="H14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="32">
+        <v>2</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="36">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="30">
+      <c r="E15" s="36"/>
+      <c r="F15" s="37">
+        <v>254</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="32"/>
+      <c r="B16" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="36">
         <v>2</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="37">
+        <v>254</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="38"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="30">
+        <v>3</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C17" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34">
-        <v>254</v>
-      </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="35"/>
-      <c r="I15">
+      <c r="D17" s="24">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="30"/>
-      <c r="B16" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34">
-        <v>254</v>
-      </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="35"/>
-      <c r="I16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="28">
-        <v>3</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23">
+      <c r="E17" s="24"/>
+      <c r="F17" s="25">
         <v>260</v>
       </c>
-      <c r="F17" s="22"/>
       <c r="G17" s="24"/>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="29"/>
+      <c r="H17" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="31"/>
       <c r="B18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="31">
+      <c r="D18" s="21">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="34">
         <v>260</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="32"/>
-      <c r="I18">
+      <c r="G18" s="21"/>
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="32">
+        <v>4</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="36">
+        <v>3</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37">
+        <v>298</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A20" s="32"/>
+      <c r="B20" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="36">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="30">
-        <v>4</v>
-      </c>
-      <c r="B19" s="33" t="s">
+      <c r="E20" s="36"/>
+      <c r="F20" s="37">
+        <v>298</v>
+      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="30">
+        <v>5</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C21" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34">
-        <v>298</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="35"/>
-      <c r="I19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="30"/>
-      <c r="B20" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34">
-        <v>298</v>
-      </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="35"/>
-      <c r="I20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="28">
-        <v>5</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="23">
+      <c r="D21" s="24">
+        <v>2</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25">
         <v>237</v>
       </c>
-      <c r="F21" s="22"/>
       <c r="G21" s="24"/>
-      <c r="I21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="29"/>
+      <c r="H21" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A22" s="31"/>
       <c r="B22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="31">
+      <c r="D22" s="21">
+        <v>2</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="34">
         <v>237</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="32"/>
-      <c r="I22">
+      <c r="G22" s="21"/>
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="32">
+        <v>6</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="36">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="30">
-        <v>6</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34">
+      <c r="E23" s="36"/>
+      <c r="F23" s="37">
         <v>189</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="35"/>
-      <c r="I23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="29"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A24" s="31"/>
       <c r="B24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="31">
+      <c r="D24" s="21">
+        <v>1</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="34">
         <v>189</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="32"/>
-      <c r="I24">
-        <v>1</v>
+      <c r="G24" s="21"/>
+      <c r="H24" s="35"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1589,5 +2191,342 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32372A5-CB46-4719-AE6C-EB285C769064}">
+  <dimension ref="B2:J48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="5" max="5" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.62890625" customWidth="1"/>
+    <col min="7" max="7" width="17.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.20703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="23">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="24">
+        <v>2</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="24">
+        <v>357</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="42">
+        <v>2</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="36">
+        <v>327</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="42">
+        <v>3</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="36">
+        <v>333</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="42">
+        <v>4</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="36">
+        <v>339</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="42">
+        <v>5</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="36">
+        <v>312</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="42">
+        <v>6</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="36">
+        <v>319</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="42">
+        <v>7</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="36">
+        <v>324</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="42">
+        <v>8</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="36">
+        <v>315</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="42">
+        <v>9</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="36">
+        <v>308</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="41">
+        <v>10</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="21">
+        <v>338</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="33"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="33"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New banana info and images and their mass, top view
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27AACA5-EEF4-474D-8F03-F9D5BA37434D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5168F818-9331-4631-B78F-B334DF29BE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="2" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Apple" sheetId="2" r:id="rId2"/>
     <sheet name="Orange" sheetId="3" r:id="rId3"/>
+    <sheet name="Banana" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="97">
   <si>
     <t>apple</t>
   </si>
@@ -158,6 +159,12 @@
   </si>
   <si>
     <t>date:24-sept-22</t>
+  </si>
+  <si>
+    <t>ver3</t>
+  </si>
+  <si>
+    <t>ver2</t>
   </si>
   <si>
     <t>photo_ver (best)</t>
@@ -485,6 +492,39 @@
   </si>
   <si>
     <t>orange10_338gram.jpg</t>
+  </si>
+  <si>
+    <t>date:26-sept-22</t>
+  </si>
+  <si>
+    <t>using cylinder volume equation</t>
+  </si>
+  <si>
+    <t>banana1_153grams_ver3.jpg</t>
+  </si>
+  <si>
+    <t>banana2_145grams_ver3.jpg</t>
+  </si>
+  <si>
+    <t>banana3_139grams_ver2.jpg</t>
+  </si>
+  <si>
+    <t>banana4_139grams_ver2.jpg</t>
+  </si>
+  <si>
+    <t>banana5_171grams_ver5.jpg</t>
+  </si>
+  <si>
+    <t>ver5</t>
+  </si>
+  <si>
+    <t>banana6_144grams_ver13.jpg</t>
+  </si>
+  <si>
+    <t>ver13</t>
+  </si>
+  <si>
+    <t>banana7_170grams_ver2.jpg</t>
   </si>
 </sst>
 </file>
@@ -1244,6 +1284,187 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="266700" y="8751570"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>605790</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>150495</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>135255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F7A79D6-6756-2B96-DCC8-3B806789B89E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="605790" y="3333750"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>262890</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>24765</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEB07D45-5D43-D608-9A56-320F6BB56FEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6899910" y="3356610"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>636270</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>120015</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD9C6E4B-48E9-E637-803A-122FCBF2342C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="636270" y="8073390"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>59055</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D6DF6A9-AE80-87DF-C0C2-9E93920B11B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6934200" y="8157210"/>
           <a:ext cx="6181725" cy="4676775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1903,7 +2124,7 @@
         <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1917,7 +2138,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>31</v>
@@ -1926,10 +2147,10 @@
         <v>37</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1951,7 +2172,7 @@
       </c>
       <c r="G13" s="24"/>
       <c r="H13" s="26" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1991,7 +2212,7 @@
       </c>
       <c r="G15" s="36"/>
       <c r="H15" s="38" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2031,7 +2252,7 @@
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2071,7 +2292,7 @@
       </c>
       <c r="G19" s="36"/>
       <c r="H19" s="24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2111,7 +2332,7 @@
       </c>
       <c r="G21" s="24"/>
       <c r="H21" s="26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2151,7 +2372,7 @@
       </c>
       <c r="G23" s="36"/>
       <c r="H23" s="38" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2174,10 +2395,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2199,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32372A5-CB46-4719-AE6C-EB285C769064}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2220,7 +2441,7 @@
         <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2234,7 +2455,7 @@
         <v>34</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>31</v>
@@ -2243,10 +2464,10 @@
         <v>37</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2263,16 +2484,16 @@
         <v>2</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G4" s="24">
         <v>357</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2287,16 +2508,16 @@
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="37" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G5" s="36">
         <v>327</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2311,16 +2532,16 @@
       </c>
       <c r="E6" s="36"/>
       <c r="F6" s="37" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G6" s="36">
         <v>333</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2335,16 +2556,16 @@
       </c>
       <c r="E7" s="36"/>
       <c r="F7" s="37" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G7" s="36">
         <v>339</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2359,16 +2580,16 @@
       </c>
       <c r="E8" s="36"/>
       <c r="F8" s="37" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G8" s="36">
         <v>312</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2383,16 +2604,16 @@
       </c>
       <c r="E9" s="36"/>
       <c r="F9" s="37" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G9" s="36">
         <v>319</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2407,16 +2628,16 @@
       </c>
       <c r="E10" s="36"/>
       <c r="F10" s="37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G10" s="36">
         <v>324</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2431,19 +2652,19 @@
       </c>
       <c r="E11" s="36"/>
       <c r="F11" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G11" s="36">
         <v>315</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I11" s="43" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2458,16 +2679,16 @@
       </c>
       <c r="E12" s="36"/>
       <c r="F12" s="37" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G12" s="36">
         <v>308</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2482,16 +2703,16 @@
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G13" s="21">
         <v>338</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2516,13 +2737,267 @@
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" t="s">
-        <v>68</v>
-      </c>
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF830D0B-08F6-45E3-BE4C-20D60B51B25E}">
+  <dimension ref="B2:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="13.3125" customWidth="1"/>
+    <col min="5" max="5" width="22.1015625" customWidth="1"/>
+    <col min="6" max="6" width="29.734375" customWidth="1"/>
+    <col min="7" max="7" width="18.3671875" customWidth="1"/>
+    <col min="8" max="8" width="25.578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.89453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="23">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="24">
+        <v>153</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="42">
+        <v>2</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="36">
+        <v>145</v>
+      </c>
+      <c r="H5" s="37"/>
+      <c r="I5" s="36"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="42">
+        <v>3</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="36">
+        <v>139</v>
+      </c>
+      <c r="H6" s="37"/>
+      <c r="I6" s="36"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="42">
+        <v>4</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="36">
+        <v>139</v>
+      </c>
+      <c r="H7" s="37"/>
+      <c r="I7" s="36"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="42">
+        <v>5</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="36">
+        <v>171</v>
+      </c>
+      <c r="H8" s="37"/>
+      <c r="I8" s="36"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="42">
+        <v>6</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="36">
+        <v>144</v>
+      </c>
+      <c r="H9" s="37"/>
+      <c r="I9" s="36"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="42">
+        <v>7</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="36">
+        <v>170</v>
+      </c>
+      <c r="H10" s="37"/>
+      <c r="I10" s="36"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="42">
+        <v>8</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="36">
+        <v>166</v>
+      </c>
+      <c r="H11" s="44"/>
+      <c r="I11" s="43"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="36"/>
+    </row>
+    <row r="13" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Collected 8 banana mass and image
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5168F818-9331-4631-B78F-B334DF29BE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83310143-42A2-4320-AE22-236DD3C1F168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
   <si>
     <t>apple</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>banana7_170grams_ver2.jpg</t>
+  </si>
+  <si>
+    <t>banana8_166grams_ver3.jpg</t>
   </si>
 </sst>
 </file>
@@ -1474,6 +1477,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>26670</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>211455</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7A228E9-5ABA-90E7-99D5-CB36D93DEA74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="12759690"/>
+          <a:ext cx="6181725" cy="4676775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2000,7 +2047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -2420,7 +2467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32372A5-CB46-4719-AE6C-EB285C769064}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -2757,7 +2804,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2971,8 +3018,12 @@
       <c r="D11" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>97</v>
+      </c>
       <c r="G11" s="36">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Banana function 3 lines, left and right outer lines touching
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83310143-42A2-4320-AE22-236DD3C1F168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA73C380-ADAD-43A5-B43F-79864D09A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
@@ -2804,7 +2804,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Got the banana volume calculation done
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA73C380-ADAD-43A5-B43F-79864D09A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A1E713-A92A-4CC5-AB16-35200B158643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Banana" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="98">
   <si>
     <t>apple</t>
   </si>
@@ -920,7 +921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1007,6 +1008,36 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1014,42 +1045,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2193,15 +2188,15 @@
       <c r="F12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="38" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="30">
+      <c r="A13" s="40">
         <v>1</v>
       </c>
       <c r="B13" s="24" t="s">
@@ -2223,65 +2218,65 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="31"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="21">
         <v>1</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="34">
+      <c r="F14" s="33">
         <v>264</v>
       </c>
       <c r="G14" s="21"/>
-      <c r="H14" s="35"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="32">
+      <c r="A15" s="42">
         <v>2</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="35">
         <v>1</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37">
+      <c r="E15" s="35"/>
+      <c r="F15" s="1">
         <v>254</v>
       </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="38" t="s">
+      <c r="G15" s="35"/>
+      <c r="H15" s="36" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="32"/>
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="42"/>
+      <c r="B16" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="35">
         <v>2</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37">
+      <c r="E16" s="35"/>
+      <c r="F16" s="1">
         <v>254</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="38"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="30">
+      <c r="A17" s="40">
         <v>3</v>
       </c>
       <c r="B17" s="24" t="s">
@@ -2303,65 +2298,65 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="31"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="21">
         <v>1</v>
       </c>
       <c r="E18" s="21"/>
-      <c r="F18" s="34">
+      <c r="F18" s="33">
         <v>260</v>
       </c>
       <c r="G18" s="21"/>
-      <c r="H18" s="35"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="32">
+      <c r="A19" s="42">
         <v>4</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D19" s="35">
         <v>3</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37">
+      <c r="E19" s="35"/>
+      <c r="F19" s="1">
         <v>298</v>
       </c>
-      <c r="G19" s="36"/>
+      <c r="G19" s="35"/>
       <c r="H19" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="32"/>
-      <c r="B20" s="36" t="s">
+      <c r="A20" s="42"/>
+      <c r="B20" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="35">
         <v>1</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37">
+      <c r="E20" s="35"/>
+      <c r="F20" s="1">
         <v>298</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="22"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="30">
+      <c r="A21" s="40">
         <v>5</v>
       </c>
       <c r="B21" s="24" t="s">
@@ -2383,62 +2378,62 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="31"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="21">
         <v>2</v>
       </c>
       <c r="E22" s="21"/>
-      <c r="F22" s="34">
+      <c r="F22" s="33">
         <v>237</v>
       </c>
       <c r="G22" s="21"/>
-      <c r="H22" s="35"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="32">
+      <c r="A23" s="42">
         <v>6</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="35">
         <v>2</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37">
+      <c r="E23" s="35"/>
+      <c r="F23" s="1">
         <v>189</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="38" t="s">
+      <c r="G23" s="35"/>
+      <c r="H23" s="36" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="31"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="21">
         <v>1</v>
       </c>
       <c r="E24" s="21"/>
-      <c r="F24" s="34">
+      <c r="F24" s="33">
         <v>189</v>
       </c>
       <c r="G24" s="21"/>
-      <c r="H24" s="35"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
@@ -2450,12 +2445,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2467,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32372A5-CB46-4719-AE6C-EB285C769064}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2510,10 +2505,10 @@
       <c r="G3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="38" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2544,170 +2539,170 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="42">
+      <c r="B5" s="31">
         <v>2</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="35">
         <v>327</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="35" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="42">
+      <c r="B6" s="31">
         <v>3</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="35">
         <v>333</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="35" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="42">
+      <c r="B7" s="31">
         <v>4</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37" t="s">
+      <c r="E7" s="35"/>
+      <c r="F7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="35">
         <v>339</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="35" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="42">
+      <c r="B8" s="31">
         <v>5</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37" t="s">
+      <c r="E8" s="35"/>
+      <c r="F8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="35">
         <v>312</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="35" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="42">
+      <c r="B9" s="31">
         <v>6</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37" t="s">
+      <c r="E9" s="35"/>
+      <c r="F9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="35">
         <v>319</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="35" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="42">
+      <c r="B10" s="31">
         <v>7</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37" t="s">
+      <c r="E10" s="35"/>
+      <c r="F10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="35">
         <v>324</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="42">
+      <c r="B11" s="31">
         <v>8</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37" t="s">
+      <c r="E11" s="35"/>
+      <c r="F11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="35">
         <v>315</v>
       </c>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="39" t="s">
         <v>68</v>
       </c>
       <c r="J11" t="s">
@@ -2715,47 +2710,47 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="42">
+      <c r="B12" s="31">
         <v>9</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37" t="s">
+      <c r="E12" s="35"/>
+      <c r="F12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="35">
         <v>308</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="35" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B13" s="41">
+      <c r="B13" s="30">
         <v>10</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="33" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="21"/>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="33" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="21">
         <v>338</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="33" t="s">
         <v>84</v>
       </c>
       <c r="I13" s="21" t="s">
@@ -2763,24 +2758,24 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="33"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="33"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="s">
@@ -2804,7 +2799,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2847,10 +2842,10 @@
       <c r="G3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="38" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2877,177 +2872,179 @@
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="42">
+      <c r="B5" s="31">
         <v>2</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="35">
         <v>145</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="36"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="42">
+      <c r="B6" s="31">
         <v>3</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="35">
         <v>139</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="36"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="42">
+      <c r="B7" s="31">
         <v>4</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="35">
         <v>139</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="36"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="42">
+      <c r="B8" s="31">
         <v>5</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="35">
         <v>171</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="36"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="42">
+      <c r="B9" s="31">
         <v>6</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="35">
         <v>144</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="36"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="42">
+      <c r="B10" s="31">
         <v>7</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="35">
         <v>170</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="36"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="35"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="42">
+      <c r="B11" s="31">
         <v>8</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="35">
         <v>166</v>
       </c>
-      <c r="H11" s="44"/>
-      <c r="I11" s="43"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="39" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="36"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
-      <c r="F13" s="34"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="21"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update adjustment values for apple,orange,banana
Apple: Median = 2.31
Orange: Median = 1.67
Banana: Median = 2.205
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A1E713-A92A-4CC5-AB16-35200B158643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01257A0-BA63-4DE8-8F05-682CCEBD90C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="99">
   <si>
     <t>apple</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Fruit/Vegetable Experiment</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Alpha (Adjust sphere equation)</t>
-  </si>
-  <si>
     <t>Image_File_Path</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
   </si>
   <si>
     <t>Actual Mass (grams)</t>
-  </si>
-  <si>
-    <t>pink lady</t>
   </si>
   <si>
     <t>date:24-sept-22</t>
@@ -465,33 +456,6 @@
     </r>
   </si>
   <si>
-    <t>[1.62, 357]</t>
-  </si>
-  <si>
-    <t>[1.5, 328]</t>
-  </si>
-  <si>
-    <t>[1.81, 332]</t>
-  </si>
-  <si>
-    <t>[2.1, 340]</t>
-  </si>
-  <si>
-    <t>[1.435, 312]</t>
-  </si>
-  <si>
-    <t>[1.6, 318]</t>
-  </si>
-  <si>
-    <t>[1.92, 323]</t>
-  </si>
-  <si>
-    <t>[1.54, 309]</t>
-  </si>
-  <si>
-    <t>[1.72, 338]</t>
-  </si>
-  <si>
     <t>orange10_338gram.jpg</t>
   </si>
   <si>
@@ -529,6 +493,136 @@
   </si>
   <si>
     <t>banana8_166grams_ver3.jpg</t>
+  </si>
+  <si>
+    <t>[2.27, 166] (square bottom)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.27, 191], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.02, 170]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.02, 133], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.18, 144]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.18, 200], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1.87, 171]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[1.87, 113], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.3, 139]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.3, 156], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.05,139]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.05, 133], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2.23, 145]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2.23, 110], </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[3.1, 153]</t>
+    </r>
+  </si>
+  <si>
+    <t>Best Adjustment</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Median</t>
   </si>
 </sst>
 </file>
@@ -921,7 +1015,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1045,6 +1139,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1070,13 +1186,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>88899</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2456392</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>32807</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1114,13 +1230,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2374901</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>105832</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1453092</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:colOff>1453093</xdr:colOff>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>49740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2040,20 +2156,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="4" width="17.20703125" customWidth="1"/>
+    <col min="3" max="3" width="17.20703125" customWidth="1"/>
+    <col min="4" max="4" width="13.20703125" customWidth="1"/>
     <col min="5" max="5" width="37.26171875" customWidth="1"/>
     <col min="6" max="6" width="33.20703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.68359375" customWidth="1"/>
-    <col min="8" max="8" width="49.3671875" customWidth="1"/>
+    <col min="8" max="8" width="28.7890625" customWidth="1"/>
+    <col min="9" max="9" width="31.734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2062,396 +2180,554 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="3" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="23">
+        <v>4</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25">
+        <v>298</v>
+      </c>
+      <c r="H4" s="25">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="31">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="35">
+        <v>254</v>
+      </c>
+      <c r="H5" s="53">
+        <v>2.15</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B6" s="31">
+        <v>6</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="35">
+        <v>189</v>
+      </c>
+      <c r="H6" s="53">
+        <v>2.15</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="31">
+        <v>3</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="35"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="35">
+        <v>260</v>
+      </c>
+      <c r="H7" s="53">
+        <v>2.4750000000000001</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="31">
+        <v>1</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="35"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="35">
+        <v>264</v>
+      </c>
+      <c r="H8" s="53">
+        <v>2.78</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="30">
+        <v>5</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="21">
+        <v>237</v>
+      </c>
+      <c r="H9" s="33">
+        <v>3</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="31"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="53"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="31"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="53"/>
+    </row>
+    <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="31"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="53"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="17"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="5"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="18"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="5"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="5"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="5"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B15" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="29" t="s">
+      <c r="E15" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="40">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="24">
+        <v>3</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25">
+        <v>264</v>
+      </c>
+      <c r="G16" s="24">
+        <v>2.78</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="41"/>
+      <c r="B17" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="28" t="s">
+      <c r="D17" s="21">
+        <v>1</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="33">
+        <v>264</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="34"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="42">
+        <v>2</v>
+      </c>
+      <c r="B18" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="40">
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="35">
         <v>1</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="24">
-        <v>3</v>
-      </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25">
-        <v>264</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="41"/>
-      <c r="B14" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="21">
-        <v>1</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="33">
-        <v>264</v>
-      </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="34"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="42">
+      <c r="E18" s="35"/>
+      <c r="F18" s="1">
+        <v>254</v>
+      </c>
+      <c r="G18" s="35">
+        <v>2.15</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="42"/>
+      <c r="B19" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="35">
         <v>2</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="35">
-        <v>1</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="1">
-        <v>254</v>
-      </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="42"/>
-      <c r="B16" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="35">
-        <v>2</v>
-      </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="1">
-        <v>254</v>
-      </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="40">
-        <v>3</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="24">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25">
-        <v>260</v>
-      </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="41"/>
-      <c r="B18" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="21">
-        <v>1</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="33">
-        <v>260</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="34"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="42">
-        <v>4</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="35">
-        <v>3</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="1">
+        <v>254</v>
+      </c>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="40">
+        <v>3</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="24">
+        <v>1</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25">
+        <v>260</v>
+      </c>
+      <c r="G20" s="24">
+        <v>2.4750000000000001</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A21" s="41"/>
+      <c r="B21" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="33">
+        <v>260</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="34"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="42">
+        <v>4</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="35">
+        <v>3</v>
+      </c>
+      <c r="E22" s="35"/>
+      <c r="F22" s="1">
         <v>298</v>
       </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="42"/>
-      <c r="B20" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="35">
+      <c r="G22" s="35">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A23" s="42"/>
+      <c r="B23" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="35">
         <v>1</v>
-      </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="1">
-        <v>298</v>
-      </c>
-      <c r="G20" s="35"/>
-      <c r="H20" s="22"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="40">
-        <v>5</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="24">
-        <v>2</v>
-      </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="25">
-        <v>237</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="41"/>
-      <c r="B22" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="21">
-        <v>2</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="33">
-        <v>237</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="34"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="42">
-        <v>6</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="35">
-        <v>2</v>
       </c>
       <c r="E23" s="35"/>
       <c r="F23" s="1">
+        <v>298</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="40">
+        <v>5</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="25">
+        <v>237</v>
+      </c>
+      <c r="G24" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="41"/>
+      <c r="B25" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="21">
+        <v>2</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="33">
+        <v>237</v>
+      </c>
+      <c r="G25" s="21"/>
+      <c r="H25" s="34"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="42">
+        <v>6</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="35">
+        <v>2</v>
+      </c>
+      <c r="E26" s="35"/>
+      <c r="F26" s="1">
         <v>189</v>
       </c>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36" t="s">
+      <c r="G26" s="35">
+        <v>2.15</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A27" s="41"/>
+      <c r="B27" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="21">
+        <v>1</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="33">
+        <v>189</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="34"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F28" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="47">
+        <f>AVERAGE(G16:G27)</f>
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="F29" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="49">
+        <f>MEDIAN(G16:G26)</f>
+        <v>2.3125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="41"/>
-      <c r="B24" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="21">
-        <v>1</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="33">
-        <v>189</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="34"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" t="s">
-        <v>52</v>
+      <c r="F32" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I9">
+    <sortCondition ref="H4:H9"/>
+  </sortState>
   <mergeCells count="6">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
+  <conditionalFormatting sqref="G16:G29">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2463,7 +2739,7 @@
   <dimension ref="B2:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2480,62 +2756,60 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="24">
-        <v>2</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E4" s="24"/>
       <c r="F4" s="25" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G4" s="24">
-        <v>357</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>76</v>
+        <v>312</v>
+      </c>
+      <c r="H4" s="25">
+        <v>1.4350000000000001</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -2546,248 +2820,275 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="35"/>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G5" s="35">
         <v>327</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>77</v>
+      <c r="H5" s="1">
+        <v>1.5</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="31">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G6" s="35">
-        <v>333</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>78</v>
+        <v>308</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.54</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G7" s="35">
-        <v>339</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>79</v>
+        <v>319</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1.6</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="1" t="s">
-        <v>64</v>
+      <c r="D8" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="35">
+        <v>2</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>51</v>
       </c>
       <c r="G8" s="35">
-        <v>312</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>80</v>
+        <v>357</v>
+      </c>
+      <c r="H8" s="53">
+        <v>1.62</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="31">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>35</v>
+      <c r="D9" s="53" t="s">
+        <v>33</v>
       </c>
       <c r="E9" s="35"/>
-      <c r="F9" s="1" t="s">
-        <v>66</v>
+      <c r="F9" s="53" t="s">
+        <v>73</v>
       </c>
       <c r="G9" s="35">
-        <v>319</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>81</v>
+        <v>338</v>
+      </c>
+      <c r="H9" s="53">
+        <v>1.72</v>
       </c>
       <c r="I9" s="35" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="31">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C10" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="G10" s="35">
-        <v>324</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>82</v>
+        <v>333</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.81</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G11" s="35">
-        <v>315</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>68</v>
+        <v>324</v>
+      </c>
+      <c r="H11" s="35">
+        <v>1.92</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="31">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="35"/>
       <c r="F12" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G12" s="35">
-        <v>308</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>73</v>
+        <v>315</v>
+      </c>
+      <c r="H12" s="53">
+        <v>1.92</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="30">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="33" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="G13" s="21">
-        <v>338</v>
-      </c>
-      <c r="H13" s="33" t="s">
-        <v>84</v>
+        <v>339</v>
+      </c>
+      <c r="H13" s="33">
+        <v>2.1</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="32"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="45">
+        <f>AVERAGE(H4:H13)</f>
+        <v>1.7164999999999999</v>
+      </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B15" s="32"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="34">
+        <f>MEDIAN(H4:H13)</f>
+        <v>1.67</v>
+      </c>
       <c r="I15" s="1"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I13">
+    <sortCondition ref="H4:H13"/>
+  </sortState>
+  <conditionalFormatting sqref="H4:H15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2796,10 +3097,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF830D0B-08F6-45E3-BE4C-20D60B51B25E}">
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2817,81 +3118,89 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G4" s="24">
-        <v>153</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="24"/>
+        <v>171</v>
+      </c>
+      <c r="H4" s="25">
+        <v>1.87</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="31">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G5" s="35">
-        <v>145</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="35"/>
+        <v>170</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2.02</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="31">
@@ -2901,130 +3210,152 @@
         <v>1</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G6" s="35">
         <v>139</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="35"/>
+      <c r="H6" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G7" s="35">
-        <v>139</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="35"/>
+        <v>144</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="35">
+        <v>145</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2.23</v>
+      </c>
+      <c r="I8" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="35">
-        <v>171</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G9" s="35">
-        <v>144</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="35"/>
+        <v>166</v>
+      </c>
+      <c r="H9" s="53">
+        <v>2.27</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="31">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="G10" s="35">
-        <v>170</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="35"/>
+        <v>139</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="31">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>97</v>
+        <v>37</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>76</v>
       </c>
       <c r="G11" s="35">
-        <v>166</v>
-      </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="39" t="s">
-        <v>68</v>
+        <v>153</v>
+      </c>
+      <c r="H11" s="35">
+        <v>3.1</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -3047,7 +3378,40 @@
       <c r="H13" s="33"/>
       <c r="I13" s="21"/>
     </row>
+    <row r="14" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="G14" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="52">
+        <f>AVERAGE(H4:H11)</f>
+        <v>2.2524999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="G15" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="49">
+        <f>MEDIAN(H4:H11)</f>
+        <v>2.2050000000000001</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:I11">
+    <sortCondition ref="H4:H11"/>
+  </sortState>
+  <conditionalFormatting sqref="H4:H15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Add apple result plot images
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B041B593-7B7C-4401-A510-515363C9184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15676B3-07FC-4B1A-9147-B5A8D3D63438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Apple" sheetId="2" r:id="rId2"/>
-    <sheet name="Orange" sheetId="3" r:id="rId3"/>
-    <sheet name="Banana" sheetId="4" r:id="rId4"/>
+    <sheet name="Tables" sheetId="5" r:id="rId2"/>
+    <sheet name="Apple" sheetId="2" r:id="rId3"/>
+    <sheet name="Orange" sheetId="3" r:id="rId4"/>
+    <sheet name="Banana" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="137">
   <si>
     <t>apple</t>
   </si>
@@ -626,12 +627,123 @@
   <si>
     <t>p</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Apple1</t>
+  </si>
+  <si>
+    <t>Apple2</t>
+  </si>
+  <si>
+    <t>Apple3</t>
+  </si>
+  <si>
+    <t>Apple4</t>
+  </si>
+  <si>
+    <t>Apple5</t>
+  </si>
+  <si>
+    <t>Apple6</t>
+  </si>
+  <si>
+    <t>Orange1</t>
+  </si>
+  <si>
+    <t>Orange2</t>
+  </si>
+  <si>
+    <t>Orange3</t>
+  </si>
+  <si>
+    <t>Orange4</t>
+  </si>
+  <si>
+    <t>Orange5</t>
+  </si>
+  <si>
+    <t>Orange6</t>
+  </si>
+  <si>
+    <t>Orange7</t>
+  </si>
+  <si>
+    <t>Orange8</t>
+  </si>
+  <si>
+    <t>Orange9</t>
+  </si>
+  <si>
+    <t>Orange10</t>
+  </si>
+  <si>
+    <t>Banana1</t>
+  </si>
+  <si>
+    <t>Banana2</t>
+  </si>
+  <si>
+    <t>Banana3</t>
+  </si>
+  <si>
+    <t>Banana4</t>
+  </si>
+  <si>
+    <t>Banana5</t>
+  </si>
+  <si>
+    <t>Banana6</t>
+  </si>
+  <si>
+    <t>Banana7</t>
+  </si>
+  <si>
+    <t>Banana8</t>
+  </si>
+  <si>
+    <t>Adjustment Constant Value β</t>
+  </si>
+  <si>
+    <t>Percentage change from median</t>
+  </si>
+  <si>
+    <t>Estimated Radius (cm)</t>
+  </si>
+  <si>
+    <t>Estimated Cross Sectional Area (cm^2)</t>
+  </si>
+  <si>
+    <t>Percentage change from median β</t>
+  </si>
+  <si>
+    <t>Average (β)</t>
+  </si>
+  <si>
+    <t>Median (β)</t>
+  </si>
+  <si>
+    <t>Number of pixels per cm</t>
+  </si>
+  <si>
+    <t>Estimated Mass (grams)</t>
+  </si>
+  <si>
+    <t>Estimated Volume (cm^3)</t>
+  </si>
+  <si>
+    <t>Estimated Calories (kcal)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,8 +767,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -687,6 +812,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -1014,10 +1145,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1153,6 +1285,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1162,15 +1297,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF63BE7B"/>
+      <color rgb="FFF8696B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2157,11 +2341,745 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B597484-1236-4C87-B23A-4EAA744D8DA1}">
+  <dimension ref="B1:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="9.62890625" customWidth="1"/>
+    <col min="4" max="4" width="11.1015625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.9453125" customWidth="1"/>
+    <col min="7" max="7" width="9.20703125" customWidth="1"/>
+    <col min="8" max="8" width="9.26171875" customWidth="1"/>
+    <col min="9" max="9" width="11.41796875" customWidth="1"/>
+    <col min="10" max="10" width="13.68359375" customWidth="1"/>
+    <col min="11" max="11" width="12.9453125" customWidth="1"/>
+    <col min="12" max="12" width="26.1015625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:11" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" s="59" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="24">
+        <v>298</v>
+      </c>
+      <c r="D3" s="23">
+        <v>18</v>
+      </c>
+      <c r="E3" s="24">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="F3" s="25">
+        <v>50.86</v>
+      </c>
+      <c r="G3" s="24">
+        <v>563.51</v>
+      </c>
+      <c r="H3" s="24">
+        <v>298.66000000000003</v>
+      </c>
+      <c r="I3" s="26">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="J3" s="26">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="K3" s="60">
+        <f>(J3-$J$10)/$J$10</f>
+        <v>-0.10702702702702704</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="35">
+        <v>254</v>
+      </c>
+      <c r="D4" s="31">
+        <v>22</v>
+      </c>
+      <c r="E4" s="35">
+        <v>3.76</v>
+      </c>
+      <c r="F4" s="65">
+        <v>44.26</v>
+      </c>
+      <c r="G4" s="35">
+        <v>478.91</v>
+      </c>
+      <c r="H4" s="35">
+        <v>253.82</v>
+      </c>
+      <c r="I4" s="36">
+        <v>131.99</v>
+      </c>
+      <c r="J4" s="36">
+        <v>2.15</v>
+      </c>
+      <c r="K4" s="61">
+        <f>(J4-$J$10)/$J$10</f>
+        <v>-7.0270270270270302E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="35">
+        <v>189</v>
+      </c>
+      <c r="D5" s="31">
+        <v>21</v>
+      </c>
+      <c r="E5" s="35">
+        <v>3.09</v>
+      </c>
+      <c r="F5" s="65">
+        <v>29.99</v>
+      </c>
+      <c r="G5" s="35">
+        <v>265.61</v>
+      </c>
+      <c r="H5" s="35">
+        <v>140.77000000000001</v>
+      </c>
+      <c r="I5" s="36">
+        <v>73.2</v>
+      </c>
+      <c r="J5" s="36">
+        <v>2.15</v>
+      </c>
+      <c r="K5" s="61">
+        <f>(J5-$J$10)/$J$10</f>
+        <v>-7.0270270270270302E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="35">
+        <v>227</v>
+      </c>
+      <c r="D6" s="31">
+        <v>23</v>
+      </c>
+      <c r="E6" s="35">
+        <v>3.46</v>
+      </c>
+      <c r="F6" s="65">
+        <v>37.619999999999997</v>
+      </c>
+      <c r="G6" s="35">
+        <v>429.6</v>
+      </c>
+      <c r="H6" s="35">
+        <v>227.68</v>
+      </c>
+      <c r="I6" s="36">
+        <v>118</v>
+      </c>
+      <c r="J6" s="36">
+        <v>2.4750000000000001</v>
+      </c>
+      <c r="K6" s="61">
+        <f>(J6-$J$10)/$J$10</f>
+        <v>7.0270270270270302E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="35">
+        <v>223</v>
+      </c>
+      <c r="D7" s="31">
+        <v>18</v>
+      </c>
+      <c r="E7" s="35">
+        <v>3.31</v>
+      </c>
+      <c r="F7" s="65">
+        <v>34.369999999999997</v>
+      </c>
+      <c r="G7" s="35">
+        <v>421.39</v>
+      </c>
+      <c r="H7" s="35">
+        <v>223.33</v>
+      </c>
+      <c r="I7" s="36">
+        <v>116.14</v>
+      </c>
+      <c r="J7" s="36">
+        <v>2.78</v>
+      </c>
+      <c r="K7" s="61">
+        <f>(J7-$J$10)/$J$10</f>
+        <v>0.20216216216216207</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="21">
+        <v>213</v>
+      </c>
+      <c r="D8" s="30">
+        <v>27</v>
+      </c>
+      <c r="E8" s="21">
+        <v>3.02</v>
+      </c>
+      <c r="F8" s="33">
+        <v>28.57</v>
+      </c>
+      <c r="G8" s="21">
+        <v>401.99</v>
+      </c>
+      <c r="H8" s="21">
+        <v>213.06</v>
+      </c>
+      <c r="I8" s="34">
+        <v>110.79</v>
+      </c>
+      <c r="J8" s="34">
+        <v>3.5</v>
+      </c>
+      <c r="K8" s="62">
+        <f>(J8-$J$10)/$J$10</f>
+        <v>0.51351351351351349</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I9" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="34">
+        <f>AVERAGE(J3:J8)</f>
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I10" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="34">
+        <f>MEDIAN(J3:J8)</f>
+        <v>2.3125</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="13" spans="2:11" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="24">
+        <v>312</v>
+      </c>
+      <c r="D14" s="23">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="E14" s="60">
+        <f>(D14-$D$25)/$D$25</f>
+        <v>-0.14071856287425144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="35">
+        <v>327</v>
+      </c>
+      <c r="D15" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="61">
+        <f t="shared" ref="E15:E23" si="0">(D15-$D$25)/$D$25</f>
+        <v>-0.1017964071856287</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="35">
+        <v>308</v>
+      </c>
+      <c r="D16" s="31">
+        <v>1.54</v>
+      </c>
+      <c r="E16" s="61">
+        <f t="shared" si="0"/>
+        <v>-7.7844311377245443E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="35">
+        <v>319</v>
+      </c>
+      <c r="D17" s="31">
+        <v>1.6</v>
+      </c>
+      <c r="E17" s="61">
+        <f t="shared" si="0"/>
+        <v>-4.1916167664670566E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="35">
+        <v>357</v>
+      </c>
+      <c r="D18" s="31">
+        <v>1.62</v>
+      </c>
+      <c r="E18" s="61">
+        <f t="shared" si="0"/>
+        <v>-2.9940119760478938E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="35">
+        <v>338</v>
+      </c>
+      <c r="D19" s="31">
+        <v>1.72</v>
+      </c>
+      <c r="E19" s="61">
+        <f t="shared" si="0"/>
+        <v>2.994011976047907E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="35">
+        <v>333</v>
+      </c>
+      <c r="D20" s="31">
+        <v>1.81</v>
+      </c>
+      <c r="E20" s="61">
+        <f t="shared" si="0"/>
+        <v>8.3832335329341395E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="35">
+        <v>324</v>
+      </c>
+      <c r="D21" s="31">
+        <v>1.92</v>
+      </c>
+      <c r="E21" s="61">
+        <f t="shared" si="0"/>
+        <v>0.14970059880239522</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="35">
+        <v>315</v>
+      </c>
+      <c r="D22" s="31">
+        <v>1.92</v>
+      </c>
+      <c r="E22" s="61">
+        <f t="shared" si="0"/>
+        <v>0.14970059880239522</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="21">
+        <v>339</v>
+      </c>
+      <c r="D23" s="30">
+        <v>2.1</v>
+      </c>
+      <c r="E23" s="62">
+        <f t="shared" si="0"/>
+        <v>0.25748502994011985</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C24" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="42">
+        <f>AVERAGE(D14:D23)</f>
+        <v>1.7164999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C25" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="34">
+        <f>MEDIAN(D14:D23)</f>
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="27" spans="2:5" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B27" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="24">
+        <v>171</v>
+      </c>
+      <c r="D28" s="25">
+        <v>1.87</v>
+      </c>
+      <c r="E28" s="60">
+        <f>(D28-$D$37)/$D$37</f>
+        <v>-0.15192743764172334</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="35">
+        <v>170</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2.02</v>
+      </c>
+      <c r="E29" s="61">
+        <f t="shared" ref="E29:E35" si="1">(D29-$D$37)/$D$37</f>
+        <v>-8.3900226757369634E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="35">
+        <v>139</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E30" s="61">
+        <f t="shared" si="1"/>
+        <v>-7.0294784580498981E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="35">
+        <v>144</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E31" s="61">
+        <f t="shared" si="1"/>
+        <v>-1.1337868480725584E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="35">
+        <v>145</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2.23</v>
+      </c>
+      <c r="E32" s="61">
+        <f t="shared" si="1"/>
+        <v>1.1337868480725584E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="35">
+        <v>166</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2.27</v>
+      </c>
+      <c r="E33" s="61">
+        <f t="shared" si="1"/>
+        <v>2.9478458049886597E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="35">
+        <v>139</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E34" s="61">
+        <f t="shared" si="1"/>
+        <v>4.3083900226757253E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B35" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="35">
+        <v>153</v>
+      </c>
+      <c r="D35" s="31">
+        <v>3.1</v>
+      </c>
+      <c r="E35" s="62">
+        <f t="shared" si="1"/>
+        <v>0.40589569160997729</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C36" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="63">
+        <f>AVERAGE(D28:D35)</f>
+        <v>2.2524999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C37" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="64">
+        <f>MEDIAN(D28:D35)</f>
+        <v>2.2050000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="J3:J8">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D25">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:J10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D35">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:D37">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D37">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:E35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2181,7 +3099,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="3" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="27" t="s">
         <v>30</v>
@@ -2334,7 +3265,7 @@
         <v>237</v>
       </c>
       <c r="H9" s="33">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="I9" s="34" t="s">
         <v>43</v>
@@ -2415,12 +3346,12 @@
       <c r="H15" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="54" t="s">
+      <c r="I15" s="51" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="53">
+      <c r="A16" s="54">
         <v>1</v>
       </c>
       <c r="B16" s="24" t="s">
@@ -2444,7 +3375,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="52"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="21" t="s">
         <v>31</v>
       </c>
@@ -2462,7 +3393,7 @@
       <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="51">
+      <c r="A18" s="52">
         <v>2</v>
       </c>
       <c r="B18" s="35" t="s">
@@ -2486,7 +3417,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="51"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="35" t="s">
         <v>31</v>
       </c>
@@ -2504,7 +3435,7 @@
       <c r="H19" s="36"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="53">
+      <c r="A20" s="54">
         <v>3</v>
       </c>
       <c r="B20" s="24" t="s">
@@ -2528,7 +3459,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="52"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="21" t="s">
         <v>31</v>
       </c>
@@ -2546,7 +3477,7 @@
       <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="51">
+      <c r="A22" s="52">
         <v>4</v>
       </c>
       <c r="B22" s="35" t="s">
@@ -2570,7 +3501,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="51"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="35" t="s">
         <v>31</v>
       </c>
@@ -2588,7 +3519,7 @@
       <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="53">
+      <c r="A24" s="54">
         <v>5</v>
       </c>
       <c r="B24" s="24" t="s">
@@ -2612,7 +3543,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="52"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="21" t="s">
         <v>31</v>
       </c>
@@ -2630,7 +3561,7 @@
       <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="51">
+      <c r="A26" s="52">
         <v>6</v>
       </c>
       <c r="B26" s="35" t="s">
@@ -2654,7 +3585,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A27" s="52"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="21" t="s">
         <v>31</v>
       </c>
@@ -2739,12 +3670,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32372A5-CB46-4719-AE6C-EB285C769064}">
   <dimension ref="B2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3100,12 +4031,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF830D0B-08F6-45E3-BE4C-20D60B51B25E}">
   <dimension ref="B2:I15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G14" sqref="G14:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Add orange results, also the adjustment value
has been changed for some reason, so had to update it again
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15676B3-07FC-4B1A-9147-B5A8D3D63438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9A4783-B0A2-424C-8E55-A47228DB2D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="2382" yWindow="2382" windowWidth="7674" windowHeight="6000" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="137">
   <si>
     <t>apple</t>
   </si>
@@ -1149,7 +1149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1329,6 +1329,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2342,10 +2345,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B597484-1236-4C87-B23A-4EAA744D8DA1}">
-  <dimension ref="B1:K37"/>
+  <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2362,30 +2365,30 @@
     <col min="12" max="12" width="26.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:11" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="68" t="s">
+    <row r="1" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:12" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="68" t="s">
         <v>135</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="68" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="66" t="s">
+      <c r="I2" s="67" t="s">
         <v>136</v>
       </c>
       <c r="J2" s="59" t="s">
@@ -2395,7 +2398,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="56" t="s">
         <v>102</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>-0.10702702702702704</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="57" t="s">
         <v>103</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>-7.0270270270270302E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="57" t="s">
         <v>104</v>
       </c>
@@ -2494,7 +2497,7 @@
         <v>-7.0270270270270302E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="57" t="s">
         <v>105</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>7.0270270270270302E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="57" t="s">
         <v>106</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>0.20216216216216207</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B8" s="58" t="s">
         <v>107</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>0.51351351351351349</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I9" s="40" t="s">
         <v>131</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I10" s="40" t="s">
         <v>132</v>
       </c>
@@ -2611,191 +2614,419 @@
         <v>2.3125</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="13" spans="2:11" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="13" spans="2:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="J13" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="K13" s="59" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="24" t="s">
         <v>108</v>
       </c>
       <c r="C14" s="24">
-        <v>312</v>
-      </c>
-      <c r="D14" s="23">
-        <v>1.4350000000000001</v>
-      </c>
-      <c r="E14" s="60">
-        <f>(D14-$D$25)/$D$25</f>
-        <v>-0.14071856287425144</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+        <v>357</v>
+      </c>
+      <c r="D14" s="24">
+        <v>18</v>
+      </c>
+      <c r="E14" s="24">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="F14" s="25">
+        <v>52.95</v>
+      </c>
+      <c r="G14" s="24">
+        <v>469.55</v>
+      </c>
+      <c r="H14" s="25">
+        <v>356.86</v>
+      </c>
+      <c r="I14" s="24">
+        <v>167.72</v>
+      </c>
+      <c r="J14" s="25">
+        <v>1.62</v>
+      </c>
+      <c r="K14" s="60">
+        <f>(J14-$J$25)/$J$25</f>
+        <v>-0.16923076923076924</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="35" t="s">
         <v>109</v>
       </c>
       <c r="C15" s="35">
-        <v>327</v>
-      </c>
-      <c r="D15" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="E15" s="61">
-        <f t="shared" ref="E15:E23" si="0">(D15-$D$25)/$D$25</f>
-        <v>-0.1017964071856287</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+        <v>312</v>
+      </c>
+      <c r="D15" s="35">
+        <v>18</v>
+      </c>
+      <c r="E15" s="35">
+        <v>3.86</v>
+      </c>
+      <c r="F15" s="65">
+        <v>46.9</v>
+      </c>
+      <c r="G15" s="35">
+        <v>410.76</v>
+      </c>
+      <c r="H15" s="65">
+        <v>312.18</v>
+      </c>
+      <c r="I15" s="35">
+        <v>146.72</v>
+      </c>
+      <c r="J15" s="65">
+        <v>1.7</v>
+      </c>
+      <c r="K15" s="61">
+        <f>(J15-$J$25)/$J$25</f>
+        <v>-0.1282051282051283</v>
+      </c>
+      <c r="L15" s="65" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="35" t="s">
         <v>110</v>
       </c>
       <c r="C16" s="35">
-        <v>308</v>
-      </c>
-      <c r="D16" s="31">
-        <v>1.54</v>
-      </c>
-      <c r="E16" s="61">
-        <f t="shared" si="0"/>
-        <v>-7.7844311377245443E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>327</v>
+      </c>
+      <c r="D16" s="35">
+        <v>17</v>
+      </c>
+      <c r="E16" s="35">
+        <v>3.86</v>
+      </c>
+      <c r="F16" s="65">
+        <v>46.71</v>
+      </c>
+      <c r="G16" s="35">
+        <v>432.21</v>
+      </c>
+      <c r="H16" s="65">
+        <v>328.48</v>
+      </c>
+      <c r="I16" s="35">
+        <v>154.38999999999999</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="K16" s="61">
+        <f>(J16-$J$25)/$J$25</f>
+        <v>-7.6923076923076983E-2</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="35" t="s">
         <v>111</v>
       </c>
       <c r="C17" s="35">
-        <v>319</v>
-      </c>
-      <c r="D17" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="E17" s="61">
-        <f t="shared" si="0"/>
-        <v>-4.1916167664670566E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>308</v>
+      </c>
+      <c r="D17" s="35">
+        <v>17</v>
+      </c>
+      <c r="E17" s="35">
+        <v>3.75</v>
+      </c>
+      <c r="F17" s="65">
+        <v>44.08</v>
+      </c>
+      <c r="G17" s="35">
+        <v>405.08</v>
+      </c>
+      <c r="H17" s="65">
+        <v>307.86</v>
+      </c>
+      <c r="I17" s="35">
+        <v>144.69</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1.84</v>
+      </c>
+      <c r="K17" s="61">
+        <f>(J17-$J$25)/$J$25</f>
+        <v>-5.6410256410256453E-2</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="35" t="s">
         <v>112</v>
       </c>
       <c r="C18" s="35">
-        <v>357</v>
-      </c>
-      <c r="D18" s="31">
-        <v>1.62</v>
-      </c>
-      <c r="E18" s="61">
-        <f t="shared" si="0"/>
-        <v>-2.9940119760478938E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>319</v>
+      </c>
+      <c r="D18" s="35">
+        <v>21</v>
+      </c>
+      <c r="E18" s="35">
+        <v>3.78</v>
+      </c>
+      <c r="F18" s="65">
+        <v>44.89</v>
+      </c>
+      <c r="G18" s="35">
+        <v>420.84</v>
+      </c>
+      <c r="H18" s="65">
+        <v>319.83999999999997</v>
+      </c>
+      <c r="I18" s="35">
+        <v>150.32</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1.86</v>
+      </c>
+      <c r="K18" s="61">
+        <f>(J18-$J$25)/$J$25</f>
+        <v>-4.6153846153846191E-2</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="35" t="s">
         <v>113</v>
       </c>
       <c r="C19" s="35">
         <v>338</v>
       </c>
-      <c r="D19" s="31">
-        <v>1.72</v>
-      </c>
-      <c r="E19" s="61">
-        <f t="shared" si="0"/>
-        <v>2.994011976047907E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" s="35">
+        <v>18</v>
+      </c>
+      <c r="E19" s="35">
+        <v>3.73</v>
+      </c>
+      <c r="F19" s="65">
+        <v>43.78</v>
+      </c>
+      <c r="G19" s="35">
+        <v>444.5</v>
+      </c>
+      <c r="H19" s="65">
+        <v>337.82</v>
+      </c>
+      <c r="I19" s="35">
+        <v>158.78</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2.04</v>
+      </c>
+      <c r="K19" s="61">
+        <f>(J19-$J$25)/$J$25</f>
+        <v>4.615384615384608E-2</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="35" t="s">
         <v>114</v>
       </c>
       <c r="C20" s="35">
         <v>333</v>
       </c>
-      <c r="D20" s="31">
-        <v>1.81</v>
-      </c>
-      <c r="E20" s="61">
-        <f t="shared" si="0"/>
-        <v>8.3832335329341395E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20" s="35">
+        <v>17</v>
+      </c>
+      <c r="E20" s="35">
+        <v>3.64</v>
+      </c>
+      <c r="F20" s="65">
+        <v>41.55</v>
+      </c>
+      <c r="G20" s="35">
+        <v>439.27</v>
+      </c>
+      <c r="H20" s="65">
+        <v>333.85</v>
+      </c>
+      <c r="I20" s="35">
+        <v>156.91</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K20" s="61">
+        <f>(J20-$J$25)/$J$25</f>
+        <v>0.11794871794871793</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="35" t="s">
         <v>115</v>
       </c>
       <c r="C21" s="35">
-        <v>324</v>
-      </c>
-      <c r="D21" s="31">
-        <v>1.92</v>
-      </c>
-      <c r="E21" s="61">
-        <f t="shared" si="0"/>
-        <v>0.14970059880239522</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>315</v>
+      </c>
+      <c r="D21" s="35">
+        <v>19</v>
+      </c>
+      <c r="E21" s="35">
+        <v>3.53</v>
+      </c>
+      <c r="F21" s="65">
+        <v>39.08</v>
+      </c>
+      <c r="G21" s="35">
+        <v>413.55</v>
+      </c>
+      <c r="H21" s="65">
+        <v>314.3</v>
+      </c>
+      <c r="I21" s="35">
+        <v>147.72</v>
+      </c>
+      <c r="J21" s="35">
+        <v>2.25</v>
+      </c>
+      <c r="K21" s="61">
+        <f>(J21-$J$25)/$J$25</f>
+        <v>0.15384615384615374</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="35" t="s">
         <v>116</v>
       </c>
       <c r="C22" s="35">
-        <v>315</v>
-      </c>
-      <c r="D22" s="31">
-        <v>1.92</v>
-      </c>
-      <c r="E22" s="61">
-        <f t="shared" si="0"/>
-        <v>0.14970059880239522</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>339</v>
+      </c>
+      <c r="D22" s="35">
+        <v>17</v>
+      </c>
+      <c r="E22" s="35">
+        <v>3.49</v>
+      </c>
+      <c r="F22" s="65">
+        <v>38.17</v>
+      </c>
+      <c r="G22" s="35">
+        <v>446.98</v>
+      </c>
+      <c r="H22" s="65">
+        <v>339.7</v>
+      </c>
+      <c r="I22" s="35">
+        <v>159.66</v>
+      </c>
+      <c r="J22" s="65">
+        <v>2.52</v>
+      </c>
+      <c r="K22" s="61">
+        <f>(J22-$J$25)/$J$25</f>
+        <v>0.29230769230769221</v>
+      </c>
+      <c r="L22" s="65" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B23" s="21" t="s">
         <v>117</v>
       </c>
       <c r="C23" s="21">
-        <v>339</v>
-      </c>
-      <c r="D23" s="30">
-        <v>2.1</v>
-      </c>
-      <c r="E23" s="62">
-        <f t="shared" si="0"/>
-        <v>0.25748502994011985</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C24" s="41" t="s">
+        <v>324</v>
+      </c>
+      <c r="D23" s="21">
+        <v>20</v>
+      </c>
+      <c r="E23" s="21">
+        <v>3.38</v>
+      </c>
+      <c r="F23" s="33">
+        <v>35.909999999999997</v>
+      </c>
+      <c r="G23" s="21">
+        <v>427.31</v>
+      </c>
+      <c r="H23" s="33">
+        <v>324.76</v>
+      </c>
+      <c r="I23" s="21">
+        <v>152.63999999999999</v>
+      </c>
+      <c r="J23" s="33">
+        <v>2.64</v>
+      </c>
+      <c r="K23" s="62">
+        <f>(J23-$J$25)/$J$25</f>
+        <v>0.35384615384615381</v>
+      </c>
+      <c r="L23" s="33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I24" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="D24" s="42">
-        <f>AVERAGE(D14:D23)</f>
-        <v>1.7164999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C25" s="40" t="s">
+      <c r="J24" s="42">
+        <f>AVERAGE(J14:J23)</f>
+        <v>2.0449999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I25" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="34">
-        <f>MEDIAN(D14:D23)</f>
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="27" spans="2:5" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J25" s="34">
+        <f>MEDIAN(J14:J23)</f>
+        <v>1.9500000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="27" spans="2:12" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B27" s="55" t="s">
         <v>101</v>
       </c>
@@ -2809,7 +3040,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="56" t="s">
         <v>118</v>
       </c>
@@ -2824,7 +3055,7 @@
         <v>-0.15192743764172334</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="57" t="s">
         <v>119</v>
       </c>
@@ -2835,11 +3066,11 @@
         <v>2.02</v>
       </c>
       <c r="E29" s="61">
-        <f t="shared" ref="E29:E35" si="1">(D29-$D$37)/$D$37</f>
+        <f t="shared" ref="E29:E35" si="0">(D29-$D$37)/$D$37</f>
         <v>-8.3900226757369634E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="57" t="s">
         <v>120</v>
       </c>
@@ -2850,11 +3081,11 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="E30" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-7.0294784580498981E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="57" t="s">
         <v>121</v>
       </c>
@@ -2865,11 +3096,11 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="E31" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-1.1337868480725584E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="57" t="s">
         <v>122</v>
       </c>
@@ -2880,7 +3111,7 @@
         <v>2.23</v>
       </c>
       <c r="E32" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1337868480725584E-2</v>
       </c>
     </row>
@@ -2895,7 +3126,7 @@
         <v>2.27</v>
       </c>
       <c r="E33" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.9478458049886597E-2</v>
       </c>
     </row>
@@ -2910,7 +3141,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E34" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.3083900226757253E-2</v>
       </c>
     </row>
@@ -2925,7 +3156,7 @@
         <v>3.1</v>
       </c>
       <c r="E35" s="62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.40589569160997729</v>
       </c>
     </row>
@@ -2950,7 +3181,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="J3:J8">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2961,7 +3192,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D25">
+  <conditionalFormatting sqref="J9:J10">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2973,7 +3204,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J10">
+  <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2985,7 +3216,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="D28:D35">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2997,7 +3228,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D35">
+  <conditionalFormatting sqref="D36:D37">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3009,7 +3240,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:D37">
+  <conditionalFormatting sqref="D28:D37">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3021,7 +3252,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D37">
+  <conditionalFormatting sqref="K3:K8">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3033,7 +3264,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K8">
+  <conditionalFormatting sqref="K14:K23">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3045,7 +3276,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E23">
+  <conditionalFormatting sqref="E28:E35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3057,7 +3288,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E35">
+  <conditionalFormatting sqref="J14:J25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3078,7 +3309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3675,7 +3906,7 @@
   <dimension ref="B2:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:H15"/>
+      <selection activeCell="G4" sqref="G4:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3726,7 +3957,7 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>2</v>
@@ -3734,47 +3965,49 @@
       <c r="D4" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="24">
+        <v>2</v>
+      </c>
       <c r="F4" s="25" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G4" s="24">
-        <v>312</v>
+        <v>357</v>
       </c>
       <c r="H4" s="25">
-        <v>1.4350000000000001</v>
+        <v>1.62</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="31">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="65" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="35"/>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
+      <c r="F5" s="65" t="s">
+        <v>61</v>
       </c>
       <c r="G5" s="35">
-        <v>327</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1.5</v>
+        <v>312</v>
+      </c>
+      <c r="H5" s="65">
+        <v>1.7</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="31">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>2</v>
@@ -3784,21 +4017,21 @@
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="G6" s="35">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="H6" s="1">
-        <v>1.54</v>
+        <v>1.8</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="31">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>2</v>
@@ -3808,21 +4041,21 @@
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G7" s="35">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="H7" s="1">
-        <v>1.6</v>
+        <v>1.84</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="31">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>2</v>
@@ -3830,20 +4063,18 @@
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="35">
-        <v>2</v>
-      </c>
+      <c r="E8" s="35"/>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="G8" s="35">
-        <v>357</v>
+        <v>319</v>
       </c>
       <c r="H8" s="1">
-        <v>1.62</v>
+        <v>1.86</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -3864,7 +4095,7 @@
         <v>338</v>
       </c>
       <c r="H9" s="1">
-        <v>1.72</v>
+        <v>2.04</v>
       </c>
       <c r="I9" s="35" t="s">
         <v>72</v>
@@ -3888,7 +4119,7 @@
         <v>333</v>
       </c>
       <c r="H10" s="1">
-        <v>1.81</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="I10" s="35" t="s">
         <v>56</v>
@@ -3896,7 +4127,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>2</v>
@@ -3906,16 +4137,16 @@
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="35">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="H11" s="35">
-        <v>1.92</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>64</v>
+        <v>2.25</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>65</v>
       </c>
       <c r="J11" t="s">
         <v>66</v>
@@ -3923,31 +4154,31 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="31">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="65" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="35"/>
-      <c r="F12" s="1" t="s">
-        <v>68</v>
+      <c r="F12" s="65" t="s">
+        <v>57</v>
       </c>
       <c r="G12" s="35">
-        <v>315</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1.92</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>65</v>
+        <v>339</v>
+      </c>
+      <c r="H12" s="65">
+        <v>2.52</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="30">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>2</v>
@@ -3957,16 +4188,16 @@
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="33" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="G13" s="21">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="H13" s="33">
-        <v>2.1</v>
+        <v>2.64</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3980,7 +4211,7 @@
       </c>
       <c r="H14" s="42">
         <f>AVERAGE(H4:H13)</f>
-        <v>1.7164999999999999</v>
+        <v>2.0449999999999999</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -3995,7 +4226,7 @@
       </c>
       <c r="H15" s="34">
         <f>MEDIAN(H4:H13)</f>
-        <v>1.67</v>
+        <v>1.9500000000000002</v>
       </c>
       <c r="I15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add banana results, once again the adjustment value
changed for some reason
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9A4783-B0A2-424C-8E55-A47228DB2D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14072E59-5071-4426-93C1-B4B4EA57328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2382" yWindow="2382" windowWidth="7674" windowHeight="6000" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="-3780" yWindow="4680" windowWidth="7674" windowHeight="6000" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
   <si>
     <t>apple</t>
   </si>
@@ -737,6 +737,9 @@
   </si>
   <si>
     <t>Estimated Calories (kcal)</t>
+  </si>
+  <si>
+    <t>redo</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1343,6 +1346,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2347,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B597484-1236-4C87-B23A-4EAA744D8DA1}">
   <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2529,6 +2535,9 @@
         <f>(J6-$J$10)/$J$10</f>
         <v>7.0270270270270302E-2</v>
       </c>
+      <c r="L6" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="57" t="s">
@@ -2562,6 +2571,9 @@
         <f>(J7-$J$10)/$J$10</f>
         <v>0.20216216216216207</v>
       </c>
+      <c r="L7" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="8" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B8" s="58" t="s">
@@ -2594,6 +2606,9 @@
       <c r="K8" s="62">
         <f>(J8-$J$10)/$J$10</f>
         <v>0.51351351351351349</v>
+      </c>
+      <c r="L8" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3026,17 +3041,35 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="27" spans="2:12" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B27" s="55" t="s">
+    <row r="27" spans="2:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B27" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="59" t="s">
+      <c r="D27" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="I27" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="J27" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="E27" s="59" t="s">
+      <c r="K27" s="59" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3048,11 +3081,32 @@
         <v>171</v>
       </c>
       <c r="D28" s="25">
+        <v>17</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1.85</v>
+      </c>
+      <c r="F28" s="25">
+        <v>50.09</v>
+      </c>
+      <c r="G28" s="24">
+        <v>272.64999999999998</v>
+      </c>
+      <c r="H28" s="25">
+        <v>171.77</v>
+      </c>
+      <c r="I28" s="24">
+        <v>152.87</v>
+      </c>
+      <c r="J28" s="25">
         <v>1.87</v>
       </c>
-      <c r="E28" s="60">
-        <f>(D28-$D$37)/$D$37</f>
-        <v>-0.15192743764172334</v>
+      <c r="K28" s="60">
+        <f>(J28-$J$37)/$J$37</f>
+        <v>-0.26522593320235749</v>
+      </c>
+      <c r="L28" s="25" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -3060,14 +3114,35 @@
         <v>119</v>
       </c>
       <c r="C29" s="35">
-        <v>170</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2.02</v>
-      </c>
-      <c r="E29" s="61">
-        <f t="shared" ref="E29:E35" si="0">(D29-$D$37)/$D$37</f>
-        <v>-8.3900226757369634E-2</v>
+        <v>145</v>
+      </c>
+      <c r="D29" s="65">
+        <v>18</v>
+      </c>
+      <c r="E29" s="35">
+        <v>1.64</v>
+      </c>
+      <c r="F29" s="65">
+        <v>40.119999999999997</v>
+      </c>
+      <c r="G29" s="35">
+        <v>230.34</v>
+      </c>
+      <c r="H29" s="65">
+        <v>145.12</v>
+      </c>
+      <c r="I29" s="35">
+        <v>129.15</v>
+      </c>
+      <c r="J29" s="1">
+        <v>2.23</v>
+      </c>
+      <c r="K29" s="61">
+        <f>(J29-$J$37)/$J$37</f>
+        <v>-0.12377210216110018</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -3075,14 +3150,35 @@
         <v>120</v>
       </c>
       <c r="C30" s="35">
-        <v>139</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="E30" s="61">
-        <f t="shared" si="0"/>
-        <v>-7.0294784580498981E-2</v>
+        <v>170</v>
+      </c>
+      <c r="D30" s="65">
+        <v>19</v>
+      </c>
+      <c r="E30" s="35">
+        <v>1.63</v>
+      </c>
+      <c r="F30" s="65">
+        <v>44.41</v>
+      </c>
+      <c r="G30" s="35">
+        <v>270.89999999999998</v>
+      </c>
+      <c r="H30" s="65">
+        <v>170.67</v>
+      </c>
+      <c r="I30" s="35">
+        <v>151.9</v>
+      </c>
+      <c r="J30" s="1">
+        <v>2.38</v>
+      </c>
+      <c r="K30" s="61">
+        <f>(J30-$J$37)/$J$37</f>
+        <v>-6.483300589390964E-2</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -3090,14 +3186,35 @@
         <v>121</v>
       </c>
       <c r="C31" s="35">
-        <v>144</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="E31" s="61">
-        <f t="shared" si="0"/>
-        <v>-1.1337868480725584E-2</v>
+        <v>139</v>
+      </c>
+      <c r="D31" s="65">
+        <v>18</v>
+      </c>
+      <c r="E31" s="35">
+        <v>1.61</v>
+      </c>
+      <c r="F31" s="65">
+        <v>35.86</v>
+      </c>
+      <c r="G31" s="35">
+        <v>221.59</v>
+      </c>
+      <c r="H31" s="65">
+        <v>139.6</v>
+      </c>
+      <c r="I31" s="35">
+        <v>124.25</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2.44</v>
+      </c>
+      <c r="K31" s="61">
+        <f>(J31-$J$37)/$J$37</f>
+        <v>-4.1257367387033395E-2</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -3105,83 +3222,167 @@
         <v>122</v>
       </c>
       <c r="C32" s="35">
-        <v>145</v>
-      </c>
-      <c r="D32" s="1">
-        <v>2.23</v>
-      </c>
-      <c r="E32" s="61">
-        <f t="shared" si="0"/>
-        <v>1.1337868480725584E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>166</v>
+      </c>
+      <c r="D32" s="65">
+        <v>20</v>
+      </c>
+      <c r="E32" s="35">
+        <v>1.65</v>
+      </c>
+      <c r="F32" s="65">
+        <v>38.42</v>
+      </c>
+      <c r="G32" s="35">
+        <v>263.85000000000002</v>
+      </c>
+      <c r="H32" s="65">
+        <v>166.22</v>
+      </c>
+      <c r="I32" s="35">
+        <v>147.94</v>
+      </c>
+      <c r="J32" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="K32" s="61">
+        <f>(J32-$J$37)/$J$37</f>
+        <v>4.1257367387033395E-2</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="57" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="35">
-        <v>166</v>
-      </c>
-      <c r="D33" s="1">
-        <v>2.27</v>
-      </c>
-      <c r="E33" s="61">
-        <f t="shared" si="0"/>
-        <v>2.9478458049886597E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+        <v>139</v>
+      </c>
+      <c r="D33" s="65">
+        <v>19</v>
+      </c>
+      <c r="E33" s="35">
+        <v>1.42</v>
+      </c>
+      <c r="F33" s="65">
+        <v>26.6</v>
+      </c>
+      <c r="G33" s="35">
+        <v>220.57</v>
+      </c>
+      <c r="H33" s="65">
+        <v>138.96</v>
+      </c>
+      <c r="I33" s="35">
+        <v>123.68</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="K33" s="61">
+        <f>(J33-$J$37)/$J$37</f>
+        <v>6.0903732809430358E-2</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="57" t="s">
         <v>124</v>
       </c>
       <c r="C34" s="35">
-        <v>139</v>
-      </c>
-      <c r="D34" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E34" s="61">
-        <f t="shared" si="0"/>
-        <v>4.3083900226757253E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>144</v>
+      </c>
+      <c r="D34" s="65">
+        <v>22</v>
+      </c>
+      <c r="E34" s="35">
+        <v>1.52</v>
+      </c>
+      <c r="F34" s="65">
+        <v>32.96</v>
+      </c>
+      <c r="G34" s="35">
+        <v>228.65</v>
+      </c>
+      <c r="H34" s="65">
+        <v>144.05000000000001</v>
+      </c>
+      <c r="I34" s="35">
+        <v>128.19999999999999</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="K34" s="61">
+        <f>(J34-$J$37)/$J$37</f>
+        <v>0.13948919449901767</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B35" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="35">
+      <c r="C35" s="21">
         <v>153</v>
       </c>
-      <c r="D35" s="31">
-        <v>3.1</v>
-      </c>
-      <c r="E35" s="62">
-        <f t="shared" si="0"/>
-        <v>0.40589569160997729</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C36" s="41" t="s">
+      <c r="D35" s="33">
+        <v>19</v>
+      </c>
+      <c r="E35" s="21">
+        <v>1.37</v>
+      </c>
+      <c r="F35" s="33">
+        <v>31.15</v>
+      </c>
+      <c r="G35" s="21">
+        <v>243.74</v>
+      </c>
+      <c r="H35" s="33">
+        <v>153.56</v>
+      </c>
+      <c r="I35" s="21">
+        <v>136.66999999999999</v>
+      </c>
+      <c r="J35" s="35">
+        <v>3.64</v>
+      </c>
+      <c r="K35" s="62">
+        <f>(J35-$J$37)/$J$37</f>
+        <v>0.43025540275049123</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I36" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="63">
-        <f>AVERAGE(D28:D35)</f>
-        <v>2.2524999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C37" s="40" t="s">
+      <c r="J36" s="63">
+        <f>AVERAGE(J28:J35)</f>
+        <v>2.6012499999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I37" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="D37" s="64">
-        <f>MEDIAN(D28:D35)</f>
-        <v>2.2050000000000001</v>
+      <c r="J37" s="64">
+        <f>MEDIAN(J28:J35)</f>
+        <v>2.5449999999999999</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="J3:J8">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3193,6 +3394,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:J10">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J10">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:J37">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3204,7 +3429,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="J36:J37">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3216,7 +3441,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D35">
+  <conditionalFormatting sqref="K3:K8">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3228,7 +3453,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:D37">
+  <conditionalFormatting sqref="K14:K23">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3240,7 +3465,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D37">
+  <conditionalFormatting sqref="K28:K35">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3252,8 +3477,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K8">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="J14:J25">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3264,7 +3489,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K14:K23">
+  <conditionalFormatting sqref="J28:J35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3276,19 +3501,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E35">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J14:J25">
+  <conditionalFormatting sqref="J28:J37">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3309,7 +3522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -4266,8 +4479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF830D0B-08F6-45E3-BE4C-20D60B51B25E}">
   <dimension ref="B2:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:H15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4345,7 +4558,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="31">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>1</v>
@@ -4354,24 +4567,24 @@
         <v>34</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G5" s="35">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="H5" s="1">
-        <v>2.02</v>
+        <v>2.23</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="31">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>1</v>
@@ -4383,21 +4596,21 @@
         <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G6" s="35">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="H6" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.38</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="31">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>1</v>
@@ -4406,24 +4619,24 @@
         <v>34</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G7" s="35">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H7" s="1">
-        <v>2.1800000000000002</v>
+        <v>2.44</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>1</v>
@@ -4435,21 +4648,21 @@
         <v>37</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G8" s="35">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="H8" s="1">
-        <v>2.23</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>92</v>
+        <v>2.65</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="31">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>1</v>
@@ -4458,24 +4671,24 @@
         <v>34</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G9" s="35">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="H9" s="1">
-        <v>2.27</v>
-      </c>
-      <c r="I9" s="39" t="s">
-        <v>86</v>
+        <v>2.7</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>1</v>
@@ -4484,19 +4697,19 @@
         <v>34</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G10" s="35">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="H10" s="1">
-        <v>2.2999999999999998</v>
+        <v>2.9</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.55000000000000004">
@@ -4519,7 +4732,7 @@
         <v>153</v>
       </c>
       <c r="H11" s="35">
-        <v>3.1</v>
+        <v>3.64</v>
       </c>
       <c r="I11" s="35" t="s">
         <v>93</v>
@@ -4551,7 +4764,7 @@
       </c>
       <c r="H14" s="49">
         <f>AVERAGE(H4:H11)</f>
-        <v>2.2524999999999999</v>
+        <v>2.6012499999999998</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -4560,7 +4773,7 @@
       </c>
       <c r="H15" s="46">
         <f>MEDIAN(H4:H11)</f>
-        <v>2.2050000000000001</v>
+        <v>2.5449999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redo apple results, changed the beta value again
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14072E59-5071-4426-93C1-B4B4EA57328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6608B2E5-720E-4DEA-9794-A0FB1A92B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3780" yWindow="4680" windowWidth="7674" windowHeight="6000" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="143">
   <si>
     <t>apple</t>
   </si>
@@ -739,7 +739,22 @@
     <t>Estimated Calories (kcal)</t>
   </si>
   <si>
-    <t>redo</t>
+    <t>apple3_sideview_260gram_1</t>
+  </si>
+  <si>
+    <t>apple1_sideview_264gram_3</t>
+  </si>
+  <si>
+    <t>apple5_sideview_237gram_2</t>
+  </si>
+  <si>
+    <t>apple6_sideview_189gram_2</t>
+  </si>
+  <si>
+    <t>apple2_sideview_254gram_1</t>
+  </si>
+  <si>
+    <t>apple4_sideview_298gram_3</t>
   </si>
 </sst>
 </file>
@@ -2353,8 +2368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B597484-1236-4C87-B23A-4EAA744D8DA1}">
   <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2434,7 +2449,10 @@
       </c>
       <c r="K3" s="60">
         <f>(J3-$J$10)/$J$10</f>
-        <v>-0.10702702702702704</v>
+        <v>-0.17068273092369488</v>
+      </c>
+      <c r="L3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2467,7 +2485,10 @@
       </c>
       <c r="K4" s="61">
         <f>(J4-$J$10)/$J$10</f>
-        <v>-7.0270270270270302E-2</v>
+        <v>-0.13654618473895594</v>
+      </c>
+      <c r="L4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2500,7 +2521,10 @@
       </c>
       <c r="K5" s="61">
         <f>(J5-$J$10)/$J$10</f>
-        <v>-7.0270270270270302E-2</v>
+        <v>-0.13654618473895594</v>
+      </c>
+      <c r="L5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2508,7 +2532,7 @@
         <v>105</v>
       </c>
       <c r="C6" s="35">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="D6" s="31">
         <v>23</v>
@@ -2520,20 +2544,20 @@
         <v>37.619999999999997</v>
       </c>
       <c r="G6" s="35">
-        <v>429.6</v>
+        <v>491.22</v>
       </c>
       <c r="H6" s="35">
-        <v>227.68</v>
+        <v>260.35000000000002</v>
       </c>
       <c r="I6" s="36">
-        <v>118</v>
-      </c>
-      <c r="J6" s="36">
-        <v>2.4750000000000001</v>
+        <v>135.38</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2.83</v>
       </c>
       <c r="K6" s="61">
         <f>(J6-$J$10)/$J$10</f>
-        <v>7.0270270270270302E-2</v>
+        <v>0.13654618473895574</v>
       </c>
       <c r="L6" t="s">
         <v>137</v>
@@ -2544,7 +2568,7 @@
         <v>106</v>
       </c>
       <c r="C7" s="35">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="D7" s="31">
         <v>18</v>
@@ -2556,23 +2580,23 @@
         <v>34.369999999999997</v>
       </c>
       <c r="G7" s="35">
-        <v>421.39</v>
+        <v>498.7</v>
       </c>
       <c r="H7" s="35">
-        <v>223.33</v>
+        <v>264.31</v>
       </c>
       <c r="I7" s="36">
-        <v>116.14</v>
-      </c>
-      <c r="J7" s="36">
-        <v>2.78</v>
+        <v>137.44</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3.29</v>
       </c>
       <c r="K7" s="61">
         <f>(J7-$J$10)/$J$10</f>
-        <v>0.20216216216216207</v>
+        <v>0.32128514056224888</v>
       </c>
       <c r="L7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2580,35 +2604,35 @@
         <v>107</v>
       </c>
       <c r="C8" s="21">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="D8" s="30">
         <v>27</v>
       </c>
       <c r="E8" s="21">
-        <v>3.02</v>
+        <v>3.01</v>
       </c>
       <c r="F8" s="33">
         <v>28.57</v>
       </c>
       <c r="G8" s="21">
-        <v>401.99</v>
+        <v>447.93</v>
       </c>
       <c r="H8" s="21">
-        <v>213.06</v>
+        <v>237.41</v>
       </c>
       <c r="I8" s="34">
-        <v>110.79</v>
-      </c>
-      <c r="J8" s="34">
-        <v>3.5</v>
+        <v>123.45</v>
+      </c>
+      <c r="J8" s="33">
+        <v>3.9</v>
       </c>
       <c r="K8" s="62">
         <f>(J8-$J$10)/$J$10</f>
-        <v>0.51351351351351349</v>
+        <v>0.56626506024096368</v>
       </c>
       <c r="L8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2617,7 +2641,7 @@
       </c>
       <c r="J9" s="34">
         <f>AVERAGE(J3:J8)</f>
-        <v>2.52</v>
+        <v>2.730833333333333</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2626,7 +2650,7 @@
       </c>
       <c r="J10" s="34">
         <f>MEDIAN(J3:J8)</f>
-        <v>2.3125</v>
+        <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
@@ -3381,8 +3405,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="J3:J8">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="J3:J5">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3394,7 +3418,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:J10">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3405,7 +3429,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J10">
+  <conditionalFormatting sqref="J3:J5 J9:J10">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:J37">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -3418,6 +3454,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:J37">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K8">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3429,7 +3477,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36:J37">
+  <conditionalFormatting sqref="K14:K23">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3441,7 +3489,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K8">
+  <conditionalFormatting sqref="K28:K35">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3453,8 +3501,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K14:K23">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="J14:J25">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3465,7 +3513,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28:K35">
+  <conditionalFormatting sqref="J28:J35">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3477,7 +3525,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14:J25">
+  <conditionalFormatting sqref="J28:J37">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:J8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3489,19 +3549,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J35">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J37">
+  <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3520,10 +3568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9CAF16E-CE9D-42FE-966E-DE59EE79D51D}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3538,12 +3586,12 @@
     <col min="9" max="9" width="31.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" t="s">
         <v>100</v>
       </c>
@@ -3557,7 +3605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="27" t="s">
         <v>30</v>
       </c>
@@ -3583,7 +3631,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="23">
         <v>4</v>
       </c>
@@ -3604,8 +3652,11 @@
       <c r="I4" s="26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B5" s="31">
         <v>2</v>
       </c>
@@ -3626,8 +3677,11 @@
       <c r="I5" s="36" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="31">
         <v>6</v>
       </c>
@@ -3648,8 +3702,11 @@
       <c r="I6" s="26" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B7" s="31">
         <v>3</v>
       </c>
@@ -3665,13 +3722,16 @@
         <v>260</v>
       </c>
       <c r="H7" s="1">
-        <v>2.4750000000000001</v>
+        <v>2.83</v>
       </c>
       <c r="I7" s="24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B8" s="31">
         <v>1</v>
       </c>
@@ -3687,13 +3747,16 @@
         <v>264</v>
       </c>
       <c r="H8" s="1">
-        <v>2.78</v>
+        <v>3.29</v>
       </c>
       <c r="I8" s="26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="30">
         <v>5</v>
       </c>
@@ -3709,13 +3772,16 @@
         <v>237</v>
       </c>
       <c r="H9" s="33">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="I9" s="34" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
       <c r="D10" s="35"/>
@@ -3725,7 +3791,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="35"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
       <c r="D11" s="35"/>
@@ -3735,7 +3801,7 @@
       <c r="H11" s="35"/>
       <c r="I11" s="35"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="31"/>
       <c r="C12" s="1"/>
       <c r="D12" s="35"/>
@@ -3745,7 +3811,7 @@
       <c r="H12" s="36"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="31"/>
       <c r="C13" s="1"/>
       <c r="D13" s="35"/>
@@ -3755,7 +3821,7 @@
       <c r="H13" s="36"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="31"/>
       <c r="C14" s="1"/>
       <c r="D14" s="35"/>
@@ -3765,7 +3831,7 @@
       <c r="H14" s="36"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="27" t="s">
         <v>30</v>
       </c>
@@ -3794,7 +3860,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="54">
         <v>1</v>
       </c>
@@ -3818,7 +3884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="53"/>
       <c r="B17" s="21" t="s">
         <v>31</v>
@@ -3836,7 +3902,7 @@
       <c r="G17" s="21"/>
       <c r="H17" s="34"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="52">
         <v>2</v>
       </c>
@@ -3860,7 +3926,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="52"/>
       <c r="B19" s="35" t="s">
         <v>31</v>
@@ -3878,7 +3944,7 @@
       <c r="G19" s="35"/>
       <c r="H19" s="36"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="54">
         <v>3</v>
       </c>
@@ -3901,8 +3967,11 @@
       <c r="H20" s="26" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="53"/>
       <c r="B21" s="21" t="s">
         <v>31</v>
@@ -3920,7 +3989,7 @@
       <c r="G21" s="21"/>
       <c r="H21" s="34"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="52">
         <v>4</v>
       </c>
@@ -3944,7 +4013,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23" s="52"/>
       <c r="B23" s="35" t="s">
         <v>31</v>
@@ -3962,7 +4031,7 @@
       <c r="G23" s="35"/>
       <c r="H23" s="22"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="54">
         <v>5</v>
       </c>
@@ -3986,7 +4055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="53"/>
       <c r="B25" s="21" t="s">
         <v>31</v>
@@ -4004,7 +4073,7 @@
       <c r="G25" s="21"/>
       <c r="H25" s="34"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="52">
         <v>6</v>
       </c>
@@ -4028,7 +4097,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A27" s="53"/>
       <c r="B27" s="21" t="s">
         <v>31</v>
@@ -4046,7 +4115,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="34"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="F28" s="43" t="s">
         <v>97</v>
       </c>
@@ -4055,7 +4124,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="F29" s="45" t="s">
         <v>98</v>
       </c>
@@ -4064,7 +4133,7 @@
         <v>2.3125</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Add radius cell to the main jupyter file
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6608B2E5-720E-4DEA-9794-A0FB1A92B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C315D7-2C4B-4151-8D77-554D16B223F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="142">
   <si>
     <t>apple</t>
   </si>
@@ -709,18 +709,12 @@
     <t>Adjustment Constant Value β</t>
   </si>
   <si>
-    <t>Percentage change from median</t>
-  </si>
-  <si>
     <t>Estimated Radius (cm)</t>
   </si>
   <si>
     <t>Estimated Cross Sectional Area (cm^2)</t>
   </si>
   <si>
-    <t>Percentage change from median β</t>
-  </si>
-  <si>
     <t>Average (β)</t>
   </si>
   <si>
@@ -755,6 +749,9 @@
   </si>
   <si>
     <t>apple4_sideview_298gram_3</t>
+  </si>
+  <si>
+    <t>Percentage change from median (β)</t>
   </si>
 </sst>
 </file>
@@ -2368,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B597484-1236-4C87-B23A-4EAA744D8DA1}">
   <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2395,28 +2392,28 @@
         <v>35</v>
       </c>
       <c r="D2" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="68" t="s">
-        <v>135</v>
-      </c>
       <c r="H2" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="67" t="s">
         <v>134</v>
-      </c>
-      <c r="I2" s="67" t="s">
-        <v>136</v>
       </c>
       <c r="J2" s="59" t="s">
         <v>126</v>
       </c>
       <c r="K2" s="59" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2452,7 +2449,7 @@
         <v>-0.17068273092369488</v>
       </c>
       <c r="L3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2488,7 +2485,7 @@
         <v>-0.13654618473895594</v>
       </c>
       <c r="L4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2524,7 +2521,7 @@
         <v>-0.13654618473895594</v>
       </c>
       <c r="L5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2560,7 +2557,7 @@
         <v>0.13654618473895574</v>
       </c>
       <c r="L6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2596,7 +2593,7 @@
         <v>0.32128514056224888</v>
       </c>
       <c r="L7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2632,23 +2629,23 @@
         <v>0.56626506024096368</v>
       </c>
       <c r="L8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I9" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="J9" s="34">
+        <v>129</v>
+      </c>
+      <c r="J9" s="64">
         <f>AVERAGE(J3:J8)</f>
         <v>2.730833333333333</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I10" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="J10" s="34">
+        <v>130</v>
+      </c>
+      <c r="J10" s="64">
         <f>MEDIAN(J3:J8)</f>
         <v>2.4900000000000002</v>
       </c>
@@ -2662,28 +2659,28 @@
         <v>35</v>
       </c>
       <c r="D13" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="G13" s="68" t="s">
-        <v>135</v>
-      </c>
       <c r="H13" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" s="68" t="s">
         <v>134</v>
-      </c>
-      <c r="I13" s="68" t="s">
-        <v>136</v>
       </c>
       <c r="J13" s="59" t="s">
         <v>126</v>
       </c>
       <c r="K13" s="59" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -3048,18 +3045,18 @@
     </row>
     <row r="24" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I24" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="J24" s="42">
+        <v>129</v>
+      </c>
+      <c r="J24" s="63">
         <f>AVERAGE(J14:J23)</f>
         <v>2.0449999999999999</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I25" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="J25" s="34">
+        <v>130</v>
+      </c>
+      <c r="J25" s="64">
         <f>MEDIAN(J14:J23)</f>
         <v>1.9500000000000002</v>
       </c>
@@ -3073,28 +3070,28 @@
         <v>35</v>
       </c>
       <c r="D27" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="G27" s="68" t="s">
-        <v>135</v>
-      </c>
       <c r="H27" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="I27" s="68" t="s">
         <v>134</v>
-      </c>
-      <c r="I27" s="68" t="s">
-        <v>136</v>
       </c>
       <c r="J27" s="59" t="s">
         <v>126</v>
       </c>
       <c r="K27" s="59" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -3387,7 +3384,7 @@
     </row>
     <row r="36" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I36" s="40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J36" s="63">
         <f>AVERAGE(J28:J35)</f>
@@ -3396,7 +3393,7 @@
     </row>
     <row r="37" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I37" s="40" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J37" s="64">
         <f>MEDIAN(J28:J35)</f>
@@ -3653,7 +3650,7 @@
         <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3678,7 +3675,7 @@
         <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3703,7 +3700,7 @@
         <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3728,7 +3725,7 @@
         <v>46</v>
       </c>
       <c r="J7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3753,7 +3750,7 @@
         <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3778,7 +3775,7 @@
         <v>43</v>
       </c>
       <c r="J9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3968,7 +3965,7 @@
         <v>46</v>
       </c>
       <c r="I20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
Update result images to have ticks and banana debug
</commit_message>
<xml_diff>
--- a/fruit_vegetable_info.xlsx
+++ b/fruit_vegetable_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Documents\UQ\UQ 2022 - Sixth Year\METR4911_ML_Python\MaskRCNN-Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C315D7-2C4B-4151-8D77-554D16B223F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD33011-881E-4566-B83F-321F893FCFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
+    <workbookView xWindow="342" yWindow="3006" windowWidth="7674" windowHeight="6000" activeTab="1" xr2:uid="{54FBAA27-63C1-4064-AD0E-3C44315E280C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2365,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B597484-1236-4C87-B23A-4EAA744D8DA1}">
   <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="G17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="K3" s="60">
         <f>(J3-$J$10)/$J$10</f>
-        <v>-0.17068273092369488</v>
+        <v>-0.27797202797202808</v>
       </c>
       <c r="L3" t="s">
         <v>140</v>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="K4" s="61">
         <f>(J4-$J$10)/$J$10</f>
-        <v>-0.13654618473895594</v>
+        <v>-0.24825174825174837</v>
       </c>
       <c r="L4" t="s">
         <v>139</v>
@@ -2493,35 +2493,35 @@
         <v>104</v>
       </c>
       <c r="C5" s="35">
-        <v>189</v>
+        <v>260</v>
       </c>
       <c r="D5" s="31">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" s="35">
-        <v>3.09</v>
+        <v>3.46</v>
       </c>
       <c r="F5" s="65">
-        <v>29.99</v>
+        <v>37.619999999999997</v>
       </c>
       <c r="G5" s="35">
-        <v>265.61</v>
+        <v>491.22</v>
       </c>
       <c r="H5" s="35">
-        <v>140.77000000000001</v>
+        <v>260.35000000000002</v>
       </c>
       <c r="I5" s="36">
-        <v>73.2</v>
+        <v>135.38</v>
       </c>
       <c r="J5" s="36">
-        <v>2.15</v>
+        <v>2.83</v>
       </c>
       <c r="K5" s="61">
         <f>(J5-$J$10)/$J$10</f>
-        <v>-0.13654618473895594</v>
+        <v>-1.0489510489510575E-2</v>
       </c>
       <c r="L5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2529,35 +2529,35 @@
         <v>105</v>
       </c>
       <c r="C6" s="35">
-        <v>260</v>
+        <v>189</v>
       </c>
       <c r="D6" s="31">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="35">
-        <v>3.46</v>
+        <v>3.09</v>
       </c>
       <c r="F6" s="65">
-        <v>37.619999999999997</v>
+        <v>29.99</v>
       </c>
       <c r="G6" s="35">
-        <v>491.22</v>
+        <v>357.02</v>
       </c>
       <c r="H6" s="35">
-        <v>260.35000000000002</v>
+        <v>189.22</v>
       </c>
       <c r="I6" s="36">
-        <v>135.38</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2.83</v>
+        <v>98.4</v>
+      </c>
+      <c r="J6" s="65">
+        <v>2.89</v>
       </c>
       <c r="K6" s="61">
         <f>(J6-$J$10)/$J$10</f>
-        <v>0.13654618473895574</v>
+        <v>1.0489510489510421E-2</v>
       </c>
       <c r="L6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="K7" s="61">
         <f>(J7-$J$10)/$J$10</f>
-        <v>0.32128514056224888</v>
+        <v>0.15034965034965023</v>
       </c>
       <c r="L7" t="s">
         <v>136</v>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="K8" s="62">
         <f>(J8-$J$10)/$J$10</f>
-        <v>0.56626506024096368</v>
+        <v>0.36363636363636348</v>
       </c>
       <c r="L8" t="s">
         <v>137</v>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="J9" s="64">
         <f>AVERAGE(J3:J8)</f>
-        <v>2.730833333333333</v>
+        <v>2.8541666666666665</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2647,7 +2647,7 @@
       </c>
       <c r="J10" s="64">
         <f>MEDIAN(J3:J8)</f>
-        <v>2.4900000000000002</v>
+        <v>2.8600000000000003</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
@@ -3401,6 +3401,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:L8">
+    <sortCondition ref="J3:J8"/>
+  </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="J3:J5">
     <cfRule type="colorScale" priority="18">

</xml_diff>